<commit_message>
added spreadsheets for keeping track of test progress
</commit_message>
<xml_diff>
--- a/resources/testing/games-loaded-successsfully.xlsx
+++ b/resources/testing/games-loaded-successsfully.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjrat\source\repos\Javascript\ChessKingsCouncil\resources\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F8517D-E85C-4296-91C7-6BD675CDBA57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE88F178-9674-42D7-90C7-B45104C67525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="2010" windowWidth="22485" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>9 Queen Checkmate</t>
   </si>
@@ -45,9 +45,6 @@
     <t>No pawn promo choices</t>
   </si>
   <si>
-    <t>Pawn promotions to useless pieces</t>
-  </si>
-  <si>
     <t>promo_test</t>
   </si>
   <si>
@@ -123,12 +120,6 @@
     <t>castle_test4</t>
   </si>
   <si>
-    <t>castle_test5</t>
-  </si>
-  <si>
-    <t>castle_test6</t>
-  </si>
-  <si>
     <t>check_example1</t>
   </si>
   <si>
@@ -190,6 +181,81 @@
   </si>
   <si>
     <t>super_checkmate_impossible_example</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>AQ</t>
+  </si>
+  <si>
+    <t>Black Wins with Queen and EvilMorty</t>
+  </si>
+  <si>
+    <t>Brian the dog</t>
+  </si>
+  <si>
+    <t>Future Military tech</t>
+  </si>
+  <si>
+    <t>Future war machines</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>Timberwolf and X Wing</t>
+  </si>
+  <si>
+    <t>VII</t>
+  </si>
+  <si>
+    <t>White wins 2 queen trap</t>
+  </si>
+  <si>
+    <t>game with linux penguins</t>
+  </si>
+  <si>
+    <t>new_test</t>
+  </si>
+  <si>
+    <t>pawn_hist_test</t>
+  </si>
+  <si>
+    <t>pawn_moves_test</t>
+  </si>
+  <si>
+    <t>res1</t>
+  </si>
+  <si>
+    <t>resignation</t>
+  </si>
+  <si>
+    <t>test name save</t>
+  </si>
+  <si>
+    <t>testing pawn hist again</t>
+  </si>
+  <si>
+    <t>testing saving name of game</t>
+  </si>
+  <si>
+    <t>two_queens</t>
+  </si>
+  <si>
+    <t>undefined</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -206,7 +272,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -221,7 +287,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -243,7 +309,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -522,15 +588,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A111"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67" style="1" customWidth="1"/>
+    <col min="1" max="1" width="67" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -545,547 +611,375 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>